<commit_message>
Milestone 5 dox with beta posters.  fix if you want.
</commit_message>
<xml_diff>
--- a/src/Docs/Pivot tables .xlsx
+++ b/src/Docs/Pivot tables .xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="150" windowWidth="19035" windowHeight="11655"/>
+    <workbookView xWindow="60" yWindow="150" windowWidth="19035" windowHeight="11655" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet7" sheetId="8" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="21">
   <si>
     <t>Harrison</t>
   </si>
@@ -505,25 +507,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="69200512"/>
-        <c:axId val="72442240"/>
+        <c:axId val="89667072"/>
+        <c:axId val="89668608"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="69200512"/>
+        <c:axId val="89667072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72442240"/>
+        <c:crossAx val="89668608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72442240"/>
+        <c:axId val="89668608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -531,7 +533,491 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69200512"/>
+        <c:crossAx val="89667072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:pivotSource>
+    <c:name>[Pivot tables .xlsx]Sheet2!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="21"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="22"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="23"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="24"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="25"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="26"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="27"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="28"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="29"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="30"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="31"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="32"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$4:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$4:$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>71.499999999999972</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$4:$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>49.199999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$4:$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>112.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$4:$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>102.19999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$G$4:$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="89773184"/>
+        <c:axId val="89774720"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="89773184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89774720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="89774720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89773184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -544,7 +1030,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -585,10 +1071,45 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="mlaws" refreshedDate="40630.986194675927" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="126">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:G127" sheet="Sheet1"/>
+    <worksheetSource ref="A1:G126" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Member" numFmtId="0">
@@ -799,6 +1320,93 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="mlaws" refreshedDate="40647.316397222225" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="142">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:G143" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="7">
+    <cacheField name="Member" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Harrison"/>
+        <s v="Laws"/>
+        <s v="Hatley"/>
+        <s v="Rabe"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Date" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2011-01-14T00:00:00" maxDate="2011-04-15T00:00:00"/>
+    </cacheField>
+    <cacheField name="Start Time" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T00:00:00" maxDate="1899-12-30T23:00:00"/>
+    </cacheField>
+    <cacheField name="End Time" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T00:00:00" maxDate="1900-01-01T00:00:00"/>
+    </cacheField>
+    <cacheField name="Hrs Worked" numFmtId="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="12" count="36">
+        <n v="8"/>
+        <n v="1"/>
+        <n v="3.5"/>
+        <n v="4"/>
+        <n v="10"/>
+        <n v="5"/>
+        <n v="3"/>
+        <n v="1.3"/>
+        <n v="1.1000000000000001"/>
+        <n v="1.5"/>
+        <n v="2"/>
+        <n v="0"/>
+        <n v="2.5"/>
+        <n v="1.2"/>
+        <n v="0.5"/>
+        <n v="0.9"/>
+        <n v="8.5"/>
+        <n v="1.8"/>
+        <n v="2.8"/>
+        <n v="3.8"/>
+        <n v="6"/>
+        <n v="2.4"/>
+        <n v="3.4"/>
+        <n v="0.8"/>
+        <n v="7"/>
+        <n v="1.9"/>
+        <n v="1.4"/>
+        <n v="12"/>
+        <n v="9.8000000000000007"/>
+        <n v="3.3"/>
+        <n v="9.9"/>
+        <n v="11.2"/>
+        <n v="4.8"/>
+        <n v="5.5"/>
+        <n v="6.5"/>
+        <n v="11"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Milestone" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="5" count="6">
+        <n v="0"/>
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Task" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Admin"/>
+        <s v="Coding"/>
+        <s v="Proj Mgnt"/>
+        <s v="Training"/>
+        <s v="Testing"/>
+        <s v="Modeling"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="126">
   <r>
@@ -1938,8 +2546,1291 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="142">
+  <r>
+    <x v="0"/>
+    <d v="2011-01-14T00:00:00"/>
+    <d v="1899-12-30T15:00:00"/>
+    <d v="1899-12-30T23:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-01-14T00:00:00"/>
+    <d v="1899-12-30T20:30:00"/>
+    <d v="1899-12-30T21:30:00"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-01-14T00:00:00"/>
+    <d v="1899-12-30T21:30:00"/>
+    <d v="1899-12-30T22:30:00"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-15T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T03:30:00"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-01-15T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-30T16:00:00"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-15T00:00:00"/>
+    <d v="1899-12-30T14:00:00"/>
+    <d v="1899-12-30T23:59:00"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-16T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-30T17:00:00"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-01-16T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-30T15:00:00"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-16T00:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <d v="1899-12-30T23:00:00"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-01-17T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T14:00:00"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-17T00:00:00"/>
+    <d v="1899-12-30T14:30:00"/>
+    <d v="1899-12-30T15:45:00"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-01-17T00:00:00"/>
+    <d v="1899-12-30T17:30:00"/>
+    <d v="1899-12-30T18:35:00"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-01-17T00:00:00"/>
+    <d v="1899-12-30T18:35:00"/>
+    <d v="1899-12-30T19:40:00"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-18T00:00:00"/>
+    <d v="1899-12-30T14:30:00"/>
+    <d v="1899-12-30T15:45:00"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-18T00:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <d v="1899-12-30T23:59:00"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-19T00:00:00"/>
+    <d v="1899-12-30T14:30:00"/>
+    <d v="1899-12-30T16:00:00"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-01-19T00:00:00"/>
+    <d v="1899-12-30T16:30:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-19T00:00:00"/>
+    <d v="1899-12-30T22:00:00"/>
+    <d v="1899-12-30T23:59:00"/>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-01-19T00:00:00"/>
+    <d v="1899-12-30T22:00:00"/>
+    <d v="1899-12-30T23:59:00"/>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-01-20T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T01:30:00"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-20T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T01:30:00"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-01-20T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T02:00:00"/>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-20T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-01-20T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-01-20T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-01-20T00:00:00"/>
+    <d v="1899-12-30T13:30:00"/>
+    <d v="1899-12-30T16:00:00"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-20T00:00:00"/>
+    <d v="1899-12-30T14:30:00"/>
+    <d v="1899-12-30T15:40:00"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-20T00:00:00"/>
+    <d v="1899-12-30T19:00:00"/>
+    <d v="1899-12-30T19:30:00"/>
+    <x v="14"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-20T00:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <d v="1899-12-30T23:30:00"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-21T00:00:00"/>
+    <d v="1899-12-30T08:55:00"/>
+    <d v="1899-12-30T09:45:00"/>
+    <x v="15"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-01-22T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T21:30:00"/>
+    <x v="16"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-01-22T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T21:30:00"/>
+    <x v="16"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-22T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T21:30:00"/>
+    <x v="16"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-01-22T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T21:30:00"/>
+    <x v="16"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-01-24T00:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <d v="1899-12-30T23:30:00"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-01-25T00:00:00"/>
+    <d v="1899-12-30T00:30:00"/>
+    <d v="1899-12-30T01:30:00"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-01-25T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T11:45:00"/>
+    <x v="17"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-01-25T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T11:45:00"/>
+    <x v="17"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-25T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T11:45:00"/>
+    <x v="17"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-01-25T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T11:45:00"/>
+    <x v="17"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-01-25T00:00:00"/>
+    <d v="1899-12-30T21:00:00"/>
+    <d v="1899-12-30T23:45:00"/>
+    <x v="18"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-01-25T00:00:00"/>
+    <d v="1899-12-30T21:15:00"/>
+    <d v="1899-12-30T23:45:00"/>
+    <x v="12"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-25T00:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <d v="1899-12-30T23:45:00"/>
+    <x v="19"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-01-25T00:00:00"/>
+    <d v="1899-12-30T19:00:00"/>
+    <d v="1899-12-30T20:45:00"/>
+    <x v="17"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-26T00:00:00"/>
+    <d v="1899-12-30T11:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-26T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T14:30:00"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-01-26T00:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <d v="1899-12-30T23:30:00"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-01-26T00:00:00"/>
+    <d v="1899-12-30T20:30:00"/>
+    <d v="1899-12-30T23:30:00"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-29T00:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <d v="1899-12-30T23:59:00"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-30T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T01:30:00"/>
+    <x v="9"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-01-31T00:00:00"/>
+    <d v="1899-12-30T11:30:00"/>
+    <d v="1899-12-30T12:45:00"/>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-06T00:00:00"/>
+    <d v="1899-12-30T22:00:00"/>
+    <d v="1899-12-31T00:00:00"/>
+    <x v="10"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-07T00:00:00"/>
+    <d v="1899-12-30T17:00:00"/>
+    <d v="1899-12-30T18:30:00"/>
+    <x v="9"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-02-06T00:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <d v="1899-12-30T23:59:00"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-02-07T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T02:00:00"/>
+    <x v="10"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-01-29T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-01-30T00:00:00"/>
+    <d v="1899-12-30T09:00:00"/>
+    <d v="1899-12-30T15:00:00"/>
+    <x v="20"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-02-05T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-30T18:00:00"/>
+    <x v="20"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-02-06T00:00:00"/>
+    <d v="1899-12-30T16:00:00"/>
+    <d v="1899-12-31T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-02-07T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-02-08T00:00:00"/>
+    <d v="1899-12-30T11:00:00"/>
+    <d v="1899-12-30T13:20:00"/>
+    <x v="21"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-08T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T11:30:00"/>
+    <x v="9"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-02-08T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T13:20:00"/>
+    <x v="22"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-02-08T00:00:00"/>
+    <d v="1899-12-30T21:30:00"/>
+    <d v="1899-12-30T23:59:00"/>
+    <x v="12"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-09T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T00:45:00"/>
+    <x v="23"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-02-09T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T01:00:00"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-09T00:00:00"/>
+    <d v="1899-12-30T08:45:00"/>
+    <d v="1899-12-30T09:15:00"/>
+    <x v="14"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-12T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-30T19:00:00"/>
+    <x v="24"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-12T00:00:00"/>
+    <d v="1899-12-30T14:00:00"/>
+    <d v="1899-12-30T18:00:00"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-15T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T11:45:00"/>
+    <x v="17"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-02-15T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <x v="10"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-02-15T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T11:45:00"/>
+    <x v="17"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-15T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T11:45:00"/>
+    <x v="17"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-17T00:00:00"/>
+    <d v="1899-12-30T11:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-17T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T14:15:00"/>
+    <x v="7"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-17T00:00:00"/>
+    <d v="1899-12-30T16:50:00"/>
+    <d v="1899-12-30T17:50:00"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-22T00:00:00"/>
+    <d v="1899-12-30T16:30:00"/>
+    <d v="1899-12-30T18:20:00"/>
+    <x v="25"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-23T00:00:00"/>
+    <d v="1899-12-30T21:00:00"/>
+    <d v="1899-12-30T22:20:00"/>
+    <x v="26"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-02-24T00:00:00"/>
+    <d v="1899-12-30T10:45:00"/>
+    <d v="1899-12-30T11:30:00"/>
+    <x v="23"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-02-24T00:00:00"/>
+    <d v="1899-12-30T10:45:00"/>
+    <d v="1899-12-30T11:30:00"/>
+    <x v="23"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-02-25T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T23:00:00"/>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-02-26T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-31T00:00:00"/>
+    <x v="27"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-24T00:00:00"/>
+    <d v="1899-12-30T10:45:00"/>
+    <d v="1899-12-30T11:30:00"/>
+    <x v="23"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-26T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <x v="24"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-26T00:00:00"/>
+    <d v="1899-12-30T21:00:00"/>
+    <d v="1899-12-30T22:30:00"/>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-26T00:00:00"/>
+    <d v="1899-12-30T22:30:00"/>
+    <d v="1899-12-30T23:30:00"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-27T00:00:00"/>
+    <d v="1899-12-30T01:00:00"/>
+    <d v="1899-12-30T02:00:00"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-22T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <x v="10"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-22T00:00:00"/>
+    <d v="1899-12-30T19:00:00"/>
+    <d v="1899-12-30T22:00:00"/>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-24T00:00:00"/>
+    <d v="1899-12-30T10:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <x v="10"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-24T00:00:00"/>
+    <d v="1899-12-30T17:00:00"/>
+    <d v="1899-12-30T18:30:00"/>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-27T00:00:00"/>
+    <d v="1899-12-30T01:00:00"/>
+    <d v="1899-12-30T02:00:00"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-27T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T15:00:00"/>
+    <x v="10"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-02-19T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-30T18:00:00"/>
+    <x v="20"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-02-27T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T22:45:00"/>
+    <x v="28"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-27T00:00:00"/>
+    <d v="1899-12-30T15:00:00"/>
+    <d v="1899-12-30T17:30:00"/>
+    <x v="12"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-27T00:00:00"/>
+    <d v="1899-12-30T19:30:00"/>
+    <d v="1899-12-30T22:45:00"/>
+    <x v="29"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-27T00:00:00"/>
+    <d v="1899-12-30T23:00:00"/>
+    <d v="1899-12-30T23:50:00"/>
+    <x v="15"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-02-28T00:00:00"/>
+    <d v="1899-12-30T11:00:00"/>
+    <d v="1899-12-30T11:50:00"/>
+    <x v="15"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-27T00:00:00"/>
+    <d v="1899-12-30T17:00:00"/>
+    <d v="1899-12-30T19:00:00"/>
+    <x v="10"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-27T00:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <d v="1899-12-31T00:00:00"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-28T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T03:30:00"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-02-28T00:00:00"/>
+    <d v="1899-12-30T13:20:00"/>
+    <d v="1899-12-30T14:20:00"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-03-02T00:00:00"/>
+    <d v="1899-12-30T20:00:00"/>
+    <d v="1899-12-30T22:00:00"/>
+    <x v="10"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-03-26T00:00:00"/>
+    <d v="1899-12-30T13:50:00"/>
+    <d v="1899-12-30T23:40:00"/>
+    <x v="30"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-03-26T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T16:00:00"/>
+    <x v="6"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-03-26T00:00:00"/>
+    <d v="1899-12-30T12:30:00"/>
+    <d v="1899-12-30T23:40:00"/>
+    <x v="31"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-03-26T00:00:00"/>
+    <d v="1899-12-30T12:30:00"/>
+    <d v="1899-12-30T23:40:00"/>
+    <x v="31"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-03-27T00:00:00"/>
+    <d v="1899-12-30T01:30:00"/>
+    <d v="1899-12-30T03:00:00"/>
+    <x v="9"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-03-27T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T17:45:00"/>
+    <x v="32"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-03-27T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T17:45:00"/>
+    <x v="32"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-03-27T00:00:00"/>
+    <d v="1899-12-30T15:00:00"/>
+    <d v="1899-12-30T17:45:00"/>
+    <x v="18"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-03-27T00:00:00"/>
+    <d v="1899-12-30T18:30:00"/>
+    <d v="1899-12-30T22:00:00"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-03-27T00:00:00"/>
+    <d v="1899-12-30T18:30:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <x v="33"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-03-27T00:00:00"/>
+    <d v="1899-12-30T18:30:00"/>
+    <d v="1899-12-30T23:59:00"/>
+    <x v="33"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-03-28T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T05:00:00"/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-03-27T00:00:00"/>
+    <d v="1899-12-30T01:00:00"/>
+    <d v="1899-12-30T03:00:00"/>
+    <x v="10"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-03-28T00:00:00"/>
+    <d v="1899-12-30T00:01:00"/>
+    <d v="1899-12-30T02:00:00"/>
+    <x v="10"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-03-27T00:00:00"/>
+    <d v="1899-12-30T19:15:00"/>
+    <d v="1899-12-30T20:15:00"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-03-27T00:00:00"/>
+    <d v="1899-12-30T22:00:00"/>
+    <d v="1899-12-30T23:59:00"/>
+    <x v="10"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-03-28T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T05:00:00"/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-03-28T00:00:00"/>
+    <d v="1899-12-30T17:30:00"/>
+    <d v="1899-12-30T23:59:00"/>
+    <x v="34"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-03-28T00:00:00"/>
+    <d v="1899-12-30T21:00:00"/>
+    <d v="1899-12-31T00:00:00"/>
+    <x v="6"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-03-28T00:00:00"/>
+    <d v="1899-12-30T14:00:00"/>
+    <d v="1899-12-30T17:00:00"/>
+    <x v="6"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-03-29T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T03:00:00"/>
+    <x v="6"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-03-28T00:00:00"/>
+    <d v="1899-12-30T21:00:00"/>
+    <d v="1899-12-31T00:00:00"/>
+    <x v="6"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-03-29T00:00:00"/>
+    <d v="1899-12-30T00:01:00"/>
+    <d v="1899-12-30T02:00:00"/>
+    <x v="10"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-04-02T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-31T00:00:00"/>
+    <x v="27"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-04-02T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-31T00:00:00"/>
+    <x v="27"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-04-03T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T03:00:00"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-04-03T00:00:00"/>
+    <d v="1899-12-30T00:00:00"/>
+    <d v="1899-12-30T03:00:00"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-04-03T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-30T23:00:00"/>
+    <x v="35"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-04-03T00:00:00"/>
+    <d v="1899-12-30T12:00:00"/>
+    <d v="1899-12-30T23:00:00"/>
+    <x v="35"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <d v="2011-04-09T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T16:00:00"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <d v="2011-04-09T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T16:00:00"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-04-09T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T16:00:00"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-04-09T00:00:00"/>
+    <d v="1899-12-30T13:00:00"/>
+    <d v="1899-12-30T16:00:00"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-04-12T00:00:00"/>
+    <d v="1899-12-30T21:00:00"/>
+    <d v="1899-12-30T23:00:00"/>
+    <x v="10"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-04-13T00:00:00"/>
+    <d v="1899-12-30T21:00:00"/>
+    <d v="1899-12-30T23:59:00"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-04-14T00:00:00"/>
+    <d v="1899-12-30T00:01:00"/>
+    <d v="1899-12-30T03:00:00"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <d v="2011-04-14T00:00:00"/>
+    <d v="1899-12-30T00:30:00"/>
+    <d v="1899-12-30T04:00:00"/>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2011-04-14T00:00:00"/>
+    <d v="1899-12-30T07:00:00"/>
+    <d v="1899-12-30T08:30:00"/>
+    <x v="9"/>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A4:F8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisCol" showAll="0">
@@ -2329,6 +4220,178 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A4:H6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0">
+      <items count="37">
+        <item x="11"/>
+        <item x="14"/>
+        <item x="23"/>
+        <item x="15"/>
+        <item x="1"/>
+        <item x="8"/>
+        <item x="13"/>
+        <item x="7"/>
+        <item x="26"/>
+        <item x="9"/>
+        <item x="17"/>
+        <item x="25"/>
+        <item x="10"/>
+        <item x="21"/>
+        <item x="12"/>
+        <item x="18"/>
+        <item x="6"/>
+        <item x="29"/>
+        <item x="22"/>
+        <item x="2"/>
+        <item x="19"/>
+        <item x="3"/>
+        <item x="32"/>
+        <item x="5"/>
+        <item x="33"/>
+        <item x="20"/>
+        <item x="34"/>
+        <item x="24"/>
+        <item x="0"/>
+        <item x="16"/>
+        <item x="28"/>
+        <item x="30"/>
+        <item x="4"/>
+        <item x="35"/>
+        <item x="31"/>
+        <item x="27"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="5"/>
+  </colFields>
+  <colItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Hrs Worked" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="6">
+    <chartFormat chart="0" format="27" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="28" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="29" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="30" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="31" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="5" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="32" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="5" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2616,7 +4679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2749,10 +4812,106 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G127"/>
+  <dimension ref="A4:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G127"/>
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="4" width="5" customWidth="1"/>
+    <col min="5" max="6" width="6" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="5" customWidth="1"/>
+    <col min="11" max="11" width="3" customWidth="1"/>
+    <col min="12" max="13" width="5" customWidth="1"/>
+    <col min="14" max="14" width="3" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" customWidth="1"/>
+    <col min="17" max="17" width="5" customWidth="1"/>
+    <col min="18" max="18" width="4" customWidth="1"/>
+    <col min="19" max="21" width="5" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" customWidth="1"/>
+    <col min="23" max="23" width="7.28515625" customWidth="1"/>
+    <col min="24" max="24" width="5" customWidth="1"/>
+    <col min="25" max="25" width="4" customWidth="1"/>
+    <col min="26" max="27" width="5" customWidth="1"/>
+    <col min="28" max="28" width="4" customWidth="1"/>
+    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:8">
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="6">
+        <v>69</v>
+      </c>
+      <c r="C6" s="6">
+        <v>71.499999999999972</v>
+      </c>
+      <c r="D6" s="6">
+        <v>49.199999999999996</v>
+      </c>
+      <c r="E6" s="6">
+        <v>112.5</v>
+      </c>
+      <c r="F6" s="6">
+        <v>102.19999999999999</v>
+      </c>
+      <c r="G6" s="6">
+        <v>79</v>
+      </c>
+      <c r="H6" s="6">
+        <v>483.39999999999992</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G143"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="G143" sqref="G143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5683,6 +7842,374 @@
         <v>4</v>
       </c>
     </row>
+    <row r="128" spans="1:7">
+      <c r="A128" t="s">
+        <v>3</v>
+      </c>
+      <c r="B128" s="1">
+        <v>40631</v>
+      </c>
+      <c r="C128" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="D128" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E128" s="5">
+        <v>2</v>
+      </c>
+      <c r="F128">
+        <v>5</v>
+      </c>
+      <c r="G128" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" t="s">
+        <v>3</v>
+      </c>
+      <c r="B129" s="1">
+        <v>40635</v>
+      </c>
+      <c r="C129" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D129" s="2">
+        <v>1</v>
+      </c>
+      <c r="E129" s="5">
+        <v>12</v>
+      </c>
+      <c r="F129">
+        <v>5</v>
+      </c>
+      <c r="G129" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" t="s">
+        <v>0</v>
+      </c>
+      <c r="B130" s="1">
+        <v>40635</v>
+      </c>
+      <c r="C130" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D130" s="2">
+        <v>1</v>
+      </c>
+      <c r="E130" s="5">
+        <v>12</v>
+      </c>
+      <c r="F130">
+        <v>5</v>
+      </c>
+      <c r="G130" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" t="s">
+        <v>3</v>
+      </c>
+      <c r="B131" s="1">
+        <v>40636</v>
+      </c>
+      <c r="C131" s="2">
+        <v>0</v>
+      </c>
+      <c r="D131" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="E131" s="5">
+        <v>3</v>
+      </c>
+      <c r="F131">
+        <v>5</v>
+      </c>
+      <c r="G131" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" t="s">
+        <v>0</v>
+      </c>
+      <c r="B132" s="1">
+        <v>40636</v>
+      </c>
+      <c r="C132" s="2">
+        <v>0</v>
+      </c>
+      <c r="D132" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="E132" s="5">
+        <v>3</v>
+      </c>
+      <c r="F132">
+        <v>5</v>
+      </c>
+      <c r="G132" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" t="s">
+        <v>3</v>
+      </c>
+      <c r="B133" s="1">
+        <v>40636</v>
+      </c>
+      <c r="C133" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D133" s="2">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E133" s="5">
+        <v>11</v>
+      </c>
+      <c r="F133">
+        <v>5</v>
+      </c>
+      <c r="G133" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" t="s">
+        <v>0</v>
+      </c>
+      <c r="B134" s="1">
+        <v>40636</v>
+      </c>
+      <c r="C134" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D134" s="2">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E134" s="5">
+        <v>11</v>
+      </c>
+      <c r="F134">
+        <v>5</v>
+      </c>
+      <c r="G134" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" t="s">
+        <v>0</v>
+      </c>
+      <c r="B135" s="1">
+        <v>40642</v>
+      </c>
+      <c r="C135" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D135" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E135" s="5">
+        <v>3</v>
+      </c>
+      <c r="F135">
+        <v>5</v>
+      </c>
+      <c r="G135" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" t="s">
+        <v>3</v>
+      </c>
+      <c r="B136" s="1">
+        <v>40642</v>
+      </c>
+      <c r="C136" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D136" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E136" s="5">
+        <v>3</v>
+      </c>
+      <c r="F136">
+        <v>5</v>
+      </c>
+      <c r="G136" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" t="s">
+        <v>2</v>
+      </c>
+      <c r="B137" s="1">
+        <v>40642</v>
+      </c>
+      <c r="C137" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D137" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E137" s="5">
+        <v>3</v>
+      </c>
+      <c r="F137">
+        <v>5</v>
+      </c>
+      <c r="G137" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" t="s">
+        <v>5</v>
+      </c>
+      <c r="B138" s="1">
+        <v>40642</v>
+      </c>
+      <c r="C138" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D138" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E138" s="5">
+        <v>3</v>
+      </c>
+      <c r="F138">
+        <v>5</v>
+      </c>
+      <c r="G138" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" s="1">
+        <v>40645</v>
+      </c>
+      <c r="C139" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D139" s="2">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E139" s="5">
+        <v>2</v>
+      </c>
+      <c r="F139">
+        <v>5</v>
+      </c>
+      <c r="G139" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" t="s">
+        <v>2</v>
+      </c>
+      <c r="B140" s="1">
+        <v>40646</v>
+      </c>
+      <c r="C140" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D140" s="2">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="E140" s="5">
+        <v>3</v>
+      </c>
+      <c r="F140">
+        <v>5</v>
+      </c>
+      <c r="G140" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" t="s">
+        <v>2</v>
+      </c>
+      <c r="B141" s="1">
+        <v>40647</v>
+      </c>
+      <c r="C141" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="D141" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="E141" s="5">
+        <v>3</v>
+      </c>
+      <c r="F141">
+        <v>5</v>
+      </c>
+      <c r="G141" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" t="s">
+        <v>5</v>
+      </c>
+      <c r="B142" s="1">
+        <v>40647</v>
+      </c>
+      <c r="C142" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D142" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E142" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="F142">
+        <v>5</v>
+      </c>
+      <c r="G142" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c r="A143" t="s">
+        <v>2</v>
+      </c>
+      <c r="B143" s="1">
+        <v>40647</v>
+      </c>
+      <c r="C143" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D143" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E143" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F143">
+        <v>5</v>
+      </c>
+      <c r="G143" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>